<commit_message>
Cambios de Estatus Rfq y Versions
</commit_message>
<xml_diff>
--- a/Documentacion/Quoite Temp.xlsx
+++ b/Documentacion/Quoite Temp.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Axis\Axis website\axis\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8790" activeTab="1"/>
   </bookViews>
@@ -15,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Customers!$A$1:$A$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Price Quote (Landscape)'!$A$1:$R$69</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -313,14 +318,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="166" formatCode="%* #,##0.00_);"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1054,7 +1059,7 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1129,20 +1134,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="12" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1153,16 +1158,16 @@
     <xf numFmtId="2" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1171,7 +1176,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1189,13 +1194,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="44" fontId="21" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="21" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="21" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1219,12 +1224,27 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1234,20 +1254,152 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1303,21 +1455,12 @@
     <xf numFmtId="2" fontId="12" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1377,144 +1520,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1797,7 +1802,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="78508BCF-C11E-48DE-A8DA-CAEDD59400DA" descr="cid:5E49FC4D-3FDA-4751-A575-8B34556ABF7A@attlocal.net"/>
+        <xdr:cNvPr id="23" name="78508BCF-C11E-48DE-A8DA-CAEDD59400DA" descr="cid:5E49FC4D-3FDA-4751-A575-8B34556ABF7A@attlocal.net">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2188,14 +2199,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -2203,12 +2214,12 @@
     <col min="4" max="4" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.5">
+    <row r="1" spans="1:5" ht="34.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2217,189 +2228,189 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="8.1" customHeight="1"/>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="4" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="67"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1">
+    <row r="7" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1">
+    <row r="8" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1">
+    <row r="9" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="10" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="66">
+      <c r="B10" s="72">
         <v>1157</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="11" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="12" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="69" t="s">
+      <c r="C13" s="70"/>
+      <c r="D13" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="70"/>
-    </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+      <c r="E13" s="75"/>
+    </row>
+    <row r="14" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="69" t="s">
+      <c r="C14" s="70"/>
+      <c r="D14" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="70"/>
-    </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+      <c r="E14" s="75"/>
+    </row>
+    <row r="15" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="72"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1">
+    <row r="16" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="72"/>
+      <c r="C17" s="67"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="18" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="72"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="19" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="72"/>
+      <c r="C19" s="67"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="20" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="72"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:5" s="6" customFormat="1">
+    <row r="21" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="22" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="67"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="23" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="72"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="67"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1">
+    <row r="24" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1">
+    <row r="25" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -2408,10 +2419,10 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1">
+    <row r="26" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -2419,11 +2430,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1">
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="11"/>
     </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="29" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -2431,10 +2442,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1">
+    <row r="30" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1">
+    <row r="31" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -2443,10 +2454,10 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1">
+    <row r="32" spans="1:5" s="6" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:2" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="33" spans="1:2" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -2456,23 +2467,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="4">
@@ -2500,14 +2511,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:L33"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="13"/>
@@ -2527,7 +2538,7 @@
     <col min="18" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.5" thickBot="1">
+    <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -2547,7 +2558,7 @@
       <c r="Q1" s="16"/>
       <c r="R1" s="16"/>
     </row>
-    <row r="2" spans="1:18" s="15" customFormat="1" ht="40.9" customHeight="1" thickTop="1">
+    <row r="2" spans="1:18" s="15" customFormat="1" ht="40.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="17"/>
       <c r="C2" s="18"/>
@@ -2560,16 +2571,16 @@
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="125" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="78"/>
+      <c r="N2" s="126"/>
+      <c r="O2" s="126"/>
+      <c r="P2" s="127"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="16"/>
     </row>
-    <row r="3" spans="1:18" ht="4.5" customHeight="1" thickBot="1">
+    <row r="3" spans="1:18" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="21"/>
       <c r="C3" s="18"/>
@@ -2582,17 +2593,17 @@
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="81"/>
+      <c r="M3" s="128"/>
+      <c r="N3" s="129"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="130"/>
       <c r="Q3" s="22" t="str">
         <f>Settings!$B$33</f>
         <v>Red</v>
       </c>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1">
+    <row r="4" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -2608,16 +2619,16 @@
       <c r="M4" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="149">
+      <c r="N4" s="91">
         <f ca="1">TODAY()</f>
-        <v>42784</v>
-      </c>
-      <c r="O4" s="150"/>
-      <c r="P4" s="151"/>
+        <v>43095</v>
+      </c>
+      <c r="O4" s="92"/>
+      <c r="P4" s="93"/>
       <c r="Q4" s="25"/>
       <c r="R4" s="16"/>
     </row>
-    <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -2633,16 +2644,16 @@
       <c r="M5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="152">
+      <c r="N5" s="94">
         <f ca="1">N4+30</f>
-        <v>42814</v>
-      </c>
-      <c r="O5" s="153"/>
-      <c r="P5" s="154"/>
+        <v>43125</v>
+      </c>
+      <c r="O5" s="95"/>
+      <c r="P5" s="96"/>
       <c r="Q5" s="25"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -2658,13 +2669,13 @@
       <c r="M6" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="N6" s="155"/>
-      <c r="O6" s="156"/>
-      <c r="P6" s="157"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="98"/>
+      <c r="P6" s="99"/>
       <c r="Q6" s="25"/>
       <c r="R6" s="16"/>
     </row>
-    <row r="7" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="7" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -2680,13 +2691,13 @@
       <c r="M7" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="N7" s="158"/>
-      <c r="O7" s="159"/>
-      <c r="P7" s="160"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="102"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="16"/>
     </row>
-    <row r="8" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1">
+    <row r="8" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -2706,7 +2717,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="1:18" ht="5.0999999999999996" customHeight="1" thickBot="1">
+    <row r="9" spans="1:18" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -2726,135 +2737,135 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1">
+    <row r="10" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="150" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="106"/>
+      <c r="C10" s="151"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="152"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="104" t="s">
+      <c r="I10" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="105"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="105"/>
-      <c r="M10" s="105"/>
-      <c r="N10" s="105"/>
-      <c r="O10" s="105"/>
-      <c r="P10" s="106"/>
+      <c r="J10" s="151"/>
+      <c r="K10" s="151"/>
+      <c r="L10" s="151"/>
+      <c r="M10" s="151"/>
+      <c r="N10" s="151"/>
+      <c r="O10" s="151"/>
+      <c r="P10" s="152"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="11" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="108"/>
-      <c r="C11" s="109"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="110"/>
+      <c r="B11" s="154"/>
+      <c r="C11" s="155"/>
+      <c r="D11" s="155"/>
+      <c r="E11" s="156"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
-      <c r="I11" s="85" t="s">
+      <c r="I11" s="134" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="87"/>
+      <c r="J11" s="135"/>
+      <c r="K11" s="135"/>
+      <c r="L11" s="135"/>
+      <c r="M11" s="135"/>
+      <c r="N11" s="135"/>
+      <c r="O11" s="135"/>
+      <c r="P11" s="136"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="115"/>
+      <c r="B12" s="159"/>
+      <c r="C12" s="160"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="161"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="87"/>
+      <c r="I12" s="134"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="135"/>
+      <c r="M12" s="135"/>
+      <c r="N12" s="135"/>
+      <c r="O12" s="135"/>
+      <c r="P12" s="136"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="114"/>
-      <c r="E13" s="115"/>
+      <c r="B13" s="159"/>
+      <c r="C13" s="160"/>
+      <c r="D13" s="160"/>
+      <c r="E13" s="161"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="87"/>
+      <c r="I13" s="134"/>
+      <c r="J13" s="135"/>
+      <c r="K13" s="135"/>
+      <c r="L13" s="135"/>
+      <c r="M13" s="135"/>
+      <c r="N13" s="135"/>
+      <c r="O13" s="135"/>
+      <c r="P13" s="136"/>
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117"/>
-      <c r="E14" s="118"/>
+      <c r="B14" s="162"/>
+      <c r="C14" s="163"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="164"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="87"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="135"/>
+      <c r="K14" s="135"/>
+      <c r="L14" s="135"/>
+      <c r="M14" s="135"/>
+      <c r="N14" s="135"/>
+      <c r="O14" s="135"/>
+      <c r="P14" s="136"/>
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
     </row>
-    <row r="15" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1">
+    <row r="15" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="107"/>
+      <c r="C15" s="153"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="153"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="90"/>
+      <c r="I15" s="137"/>
+      <c r="J15" s="138"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="138"/>
+      <c r="N15" s="138"/>
+      <c r="O15" s="138"/>
+      <c r="P15" s="139"/>
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
     </row>
-    <row r="16" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1">
+    <row r="16" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="65" t="s">
         <v>90</v>
@@ -2876,7 +2887,7 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
     </row>
-    <row r="17" spans="1:18" ht="5.0999999999999996" customHeight="1" thickBot="1">
+    <row r="17" spans="1:18" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2896,264 +2907,264 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
     </row>
-    <row r="18" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1">
+    <row r="18" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
-      <c r="B18" s="146" t="s">
+      <c r="B18" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="147"/>
-      <c r="D18" s="147"/>
-      <c r="E18" s="147"/>
-      <c r="F18" s="147"/>
-      <c r="G18" s="147"/>
-      <c r="H18" s="147"/>
-      <c r="I18" s="147"/>
-      <c r="J18" s="147"/>
-      <c r="K18" s="147"/>
-      <c r="L18" s="147"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
       <c r="M18" s="30" t="s">
         <v>47</v>
       </c>
       <c r="N18" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="O18" s="161" t="s">
+      <c r="O18" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="P18" s="162"/>
+      <c r="P18" s="84"/>
       <c r="Q18" s="25"/>
       <c r="R18" s="31"/>
     </row>
-    <row r="19" spans="1:18" ht="18.75">
+    <row r="19" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
-      <c r="B19" s="139" t="s">
+      <c r="B19" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
-      <c r="H19" s="148"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="148"/>
-      <c r="K19" s="148"/>
-      <c r="L19" s="148"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
+      <c r="L19" s="88"/>
       <c r="M19" s="54">
         <v>750</v>
       </c>
       <c r="N19" s="55">
         <v>2</v>
       </c>
-      <c r="O19" s="111">
+      <c r="O19" s="157">
         <f>IF(N19&gt;0,SUM(M19*N19),"TBD")</f>
         <v>1500</v>
       </c>
-      <c r="P19" s="112"/>
+      <c r="P19" s="158"/>
       <c r="Q19" s="34"/>
       <c r="R19" s="16"/>
     </row>
-    <row r="20" spans="1:18" ht="18.75">
+    <row r="20" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
-      <c r="B20" s="119" t="s">
+      <c r="B20" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
-      <c r="J20" s="120"/>
-      <c r="K20" s="120"/>
-      <c r="L20" s="120"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="90"/>
+      <c r="L20" s="90"/>
       <c r="M20" s="56">
         <v>750</v>
       </c>
       <c r="N20" s="57">
         <v>2</v>
       </c>
-      <c r="O20" s="97">
+      <c r="O20" s="81">
         <f>IF(N20&gt;0,SUM(M20*N20),"TBD")</f>
         <v>1500</v>
       </c>
-      <c r="P20" s="98"/>
+      <c r="P20" s="82"/>
       <c r="Q20" s="34"/>
       <c r="R20" s="16"/>
     </row>
-    <row r="21" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="21" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
-      <c r="B21" s="119"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="120"/>
-      <c r="J21" s="120"/>
-      <c r="K21" s="120"/>
-      <c r="L21" s="120"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="90"/>
+      <c r="L21" s="90"/>
       <c r="M21" s="54"/>
       <c r="N21" s="55"/>
-      <c r="O21" s="97"/>
-      <c r="P21" s="98"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="82"/>
       <c r="Q21" s="34"/>
       <c r="R21" s="16"/>
     </row>
-    <row r="22" spans="1:18" ht="18.75">
+    <row r="22" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
-      <c r="B22" s="119" t="s">
+      <c r="B22" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="120"/>
-      <c r="L22" s="120"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="90"/>
+      <c r="L22" s="90"/>
       <c r="M22" s="56">
         <v>75</v>
       </c>
       <c r="N22" s="57"/>
-      <c r="O22" s="97" t="str">
+      <c r="O22" s="81" t="str">
         <f>IF(N22&gt;0,SUM(M22*N22),"TBD")</f>
         <v>TBD</v>
       </c>
-      <c r="P22" s="98"/>
+      <c r="P22" s="82"/>
       <c r="Q22" s="34"/>
       <c r="R22" s="16"/>
     </row>
-    <row r="23" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="23" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
-      <c r="B23" s="139"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="94"/>
-      <c r="J23" s="94"/>
-      <c r="K23" s="94"/>
-      <c r="L23" s="94"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="103"/>
+      <c r="K23" s="103"/>
+      <c r="L23" s="103"/>
       <c r="M23" s="54"/>
       <c r="N23" s="55"/>
-      <c r="O23" s="97"/>
-      <c r="P23" s="98"/>
+      <c r="O23" s="81"/>
+      <c r="P23" s="82"/>
       <c r="Q23" s="34"/>
       <c r="R23" s="16"/>
     </row>
-    <row r="24" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="24" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
-      <c r="B24" s="91"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="92"/>
+      <c r="B24" s="140"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="141"/>
+      <c r="E24" s="141"/>
+      <c r="F24" s="141"/>
+      <c r="G24" s="141"/>
+      <c r="H24" s="141"/>
+      <c r="I24" s="141"/>
+      <c r="J24" s="141"/>
+      <c r="K24" s="141"/>
+      <c r="L24" s="141"/>
       <c r="M24" s="35"/>
       <c r="N24" s="36"/>
-      <c r="O24" s="97"/>
-      <c r="P24" s="98"/>
+      <c r="O24" s="81"/>
+      <c r="P24" s="82"/>
       <c r="Q24" s="34"/>
       <c r="R24" s="16"/>
     </row>
-    <row r="25" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="25" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="94"/>
-      <c r="J25" s="94"/>
-      <c r="K25" s="94"/>
-      <c r="L25" s="94"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="103"/>
+      <c r="J25" s="103"/>
+      <c r="K25" s="103"/>
+      <c r="L25" s="103"/>
       <c r="M25" s="32"/>
       <c r="N25" s="33"/>
-      <c r="O25" s="97"/>
-      <c r="P25" s="98"/>
+      <c r="O25" s="81"/>
+      <c r="P25" s="82"/>
       <c r="Q25" s="34"/>
       <c r="R25" s="16"/>
     </row>
-    <row r="26" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="26" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
-      <c r="B26" s="95"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-      <c r="E26" s="96"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="96"/>
-      <c r="H26" s="96"/>
-      <c r="I26" s="96"/>
-      <c r="J26" s="96"/>
-      <c r="K26" s="96"/>
-      <c r="L26" s="96"/>
+      <c r="B26" s="143"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="144"/>
+      <c r="K26" s="144"/>
+      <c r="L26" s="144"/>
       <c r="M26" s="35"/>
       <c r="N26" s="36"/>
-      <c r="O26" s="97"/>
-      <c r="P26" s="98"/>
+      <c r="O26" s="81"/>
+      <c r="P26" s="82"/>
       <c r="Q26" s="34"/>
       <c r="R26" s="16"/>
     </row>
-    <row r="27" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="27" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
-      <c r="B27" s="142" t="s">
+      <c r="B27" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="143"/>
-      <c r="D27" s="143"/>
-      <c r="E27" s="143"/>
-      <c r="F27" s="143"/>
-      <c r="G27" s="143"/>
-      <c r="H27" s="143"/>
-      <c r="I27" s="143"/>
-      <c r="J27" s="143"/>
-      <c r="K27" s="143"/>
-      <c r="L27" s="143"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="107"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="107"/>
+      <c r="L27" s="107"/>
       <c r="M27" s="32"/>
       <c r="N27" s="33"/>
-      <c r="O27" s="140"/>
-      <c r="P27" s="141"/>
+      <c r="O27" s="104"/>
+      <c r="P27" s="105"/>
       <c r="Q27" s="34"/>
       <c r="R27" s="16"/>
     </row>
-    <row r="28" spans="1:18" ht="18.600000000000001" customHeight="1" thickBot="1">
+    <row r="28" spans="1:18" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
-      <c r="B28" s="144" t="s">
+      <c r="B28" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="145"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="145"/>
-      <c r="H28" s="145"/>
-      <c r="I28" s="145"/>
-      <c r="J28" s="145"/>
-      <c r="K28" s="145"/>
-      <c r="L28" s="145"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="109"/>
+      <c r="J28" s="109"/>
+      <c r="K28" s="109"/>
+      <c r="L28" s="109"/>
       <c r="M28" s="37"/>
       <c r="N28" s="38"/>
-      <c r="O28" s="102"/>
-      <c r="P28" s="103"/>
+      <c r="O28" s="148"/>
+      <c r="P28" s="149"/>
       <c r="Q28" s="34"/>
       <c r="R28" s="16"/>
     </row>
-    <row r="29" spans="1:18" ht="16.5" thickTop="1">
+    <row r="29" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
@@ -3173,7 +3184,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" spans="1:18" s="14" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
+    <row r="30" spans="1:18" s="14" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="40"/>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
@@ -3193,21 +3204,21 @@
       <c r="Q30" s="40"/>
       <c r="R30" s="40"/>
     </row>
-    <row r="31" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1">
+    <row r="31" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
-      <c r="B31" s="99" t="s">
+      <c r="B31" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="100"/>
-      <c r="H31" s="100"/>
-      <c r="I31" s="100"/>
-      <c r="J31" s="100"/>
-      <c r="K31" s="100"/>
-      <c r="L31" s="101"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
+      <c r="H31" s="146"/>
+      <c r="I31" s="146"/>
+      <c r="J31" s="146"/>
+      <c r="K31" s="146"/>
+      <c r="L31" s="147"/>
       <c r="M31" s="16"/>
       <c r="N31" s="43"/>
       <c r="O31" s="43" t="str">
@@ -3218,64 +3229,64 @@
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
     </row>
-    <row r="32" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1">
+    <row r="32" spans="1:18" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
-      <c r="B32" s="125" t="s">
+      <c r="B32" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="126"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="126"/>
-      <c r="F32" s="126"/>
-      <c r="G32" s="126"/>
-      <c r="H32" s="126"/>
-      <c r="I32" s="126"/>
-      <c r="J32" s="126"/>
-      <c r="K32" s="126"/>
-      <c r="L32" s="127"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="115"/>
+      <c r="J32" s="115"/>
+      <c r="K32" s="115"/>
+      <c r="L32" s="116"/>
       <c r="M32" s="16"/>
       <c r="N32" s="43"/>
-      <c r="O32" s="121">
+      <c r="O32" s="110">
         <f>IF(SUM(O19:P28)&lt;1,"TBD",(SUM(O19:P28)))</f>
         <v>3000</v>
       </c>
-      <c r="P32" s="122"/>
+      <c r="P32" s="111"/>
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
     </row>
-    <row r="33" spans="1:18" ht="38.450000000000003" customHeight="1" thickTop="1">
+    <row r="33" spans="1:18" ht="38.450000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
-      <c r="B33" s="128"/>
-      <c r="C33" s="129"/>
-      <c r="D33" s="129"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="129"/>
-      <c r="G33" s="129"/>
-      <c r="H33" s="129"/>
-      <c r="I33" s="129"/>
-      <c r="J33" s="129"/>
-      <c r="K33" s="129"/>
-      <c r="L33" s="130"/>
+      <c r="B33" s="117"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="118"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="118"/>
+      <c r="K33" s="118"/>
+      <c r="L33" s="119"/>
       <c r="M33" s="16"/>
       <c r="N33" s="43"/>
-      <c r="O33" s="163"/>
-      <c r="P33" s="163"/>
+      <c r="O33" s="77"/>
+      <c r="P33" s="77"/>
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
     </row>
-    <row r="34" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
-      <c r="B34" s="82"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="83"/>
-      <c r="H34" s="83"/>
-      <c r="I34" s="83"/>
-      <c r="J34" s="83"/>
-      <c r="K34" s="83"/>
-      <c r="L34" s="84"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="132"/>
+      <c r="D34" s="132"/>
+      <c r="E34" s="132"/>
+      <c r="F34" s="132"/>
+      <c r="G34" s="132"/>
+      <c r="H34" s="132"/>
+      <c r="I34" s="132"/>
+      <c r="J34" s="132"/>
+      <c r="K34" s="132"/>
+      <c r="L34" s="133"/>
       <c r="M34" s="16"/>
       <c r="N34" s="43"/>
       <c r="O34" s="43" t="str">
@@ -3286,19 +3297,19 @@
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
-      <c r="B35" s="132"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="133"/>
-      <c r="E35" s="133"/>
-      <c r="F35" s="133"/>
-      <c r="G35" s="133"/>
-      <c r="H35" s="133"/>
-      <c r="I35" s="133"/>
-      <c r="J35" s="133"/>
-      <c r="K35" s="133"/>
-      <c r="L35" s="134"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="121"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="121"/>
+      <c r="F35" s="121"/>
+      <c r="G35" s="121"/>
+      <c r="H35" s="121"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="121"/>
+      <c r="K35" s="121"/>
+      <c r="L35" s="122"/>
       <c r="M35" s="16"/>
       <c r="N35" s="46"/>
       <c r="O35" s="47" t="str">
@@ -3309,7 +3320,7 @@
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
     </row>
-    <row r="36" spans="1:18" ht="5.0999999999999996" customHeight="1" thickTop="1">
+    <row r="36" spans="1:18" ht="5.0999999999999996" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -3329,51 +3340,51 @@
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
     </row>
-    <row r="37" spans="1:18" ht="15.75">
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
-      <c r="B37" s="123" t="s">
+      <c r="B37" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="123"/>
-      <c r="D37" s="123"/>
-      <c r="E37" s="123"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="123"/>
-      <c r="H37" s="123"/>
-      <c r="I37" s="123"/>
-      <c r="J37" s="123"/>
-      <c r="K37" s="123"/>
-      <c r="L37" s="123"/>
-      <c r="M37" s="123"/>
-      <c r="N37" s="123"/>
-      <c r="O37" s="123"/>
-      <c r="P37" s="123"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="112"/>
+      <c r="G37" s="112"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="112"/>
+      <c r="J37" s="112"/>
+      <c r="K37" s="112"/>
+      <c r="L37" s="112"/>
+      <c r="M37" s="112"/>
+      <c r="N37" s="112"/>
+      <c r="O37" s="112"/>
+      <c r="P37" s="112"/>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
     </row>
-    <row r="38" spans="1:18" ht="15.75">
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
-      <c r="B38" s="123" t="s">
+      <c r="B38" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="123"/>
-      <c r="D38" s="123"/>
-      <c r="E38" s="123"/>
-      <c r="F38" s="123"/>
-      <c r="G38" s="123"/>
-      <c r="H38" s="123"/>
-      <c r="I38" s="123"/>
-      <c r="J38" s="123"/>
-      <c r="K38" s="123"/>
-      <c r="L38" s="123"/>
-      <c r="M38" s="123"/>
-      <c r="N38" s="123"/>
-      <c r="O38" s="123"/>
-      <c r="P38" s="123"/>
+      <c r="C38" s="112"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="112"/>
+      <c r="H38" s="112"/>
+      <c r="I38" s="112"/>
+      <c r="J38" s="112"/>
+      <c r="K38" s="112"/>
+      <c r="L38" s="112"/>
+      <c r="M38" s="112"/>
+      <c r="N38" s="112"/>
+      <c r="O38" s="112"/>
+      <c r="P38" s="112"/>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
     </row>
-    <row r="39" spans="1:18" ht="5.0999999999999996" customHeight="1">
+    <row r="39" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -3393,7 +3404,7 @@
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
     </row>
-    <row r="40" spans="1:18" ht="15.75">
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -3413,7 +3424,7 @@
       <c r="Q40" s="16"/>
       <c r="R40" s="16"/>
     </row>
-    <row r="41" spans="1:18" ht="12.95" customHeight="1">
+    <row r="41" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="63" t="s">
         <v>49</v>
@@ -3435,7 +3446,7 @@
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
     </row>
-    <row r="42" spans="1:18" ht="12.95" customHeight="1">
+    <row r="42" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="39"/>
       <c r="C42" s="16"/>
@@ -3455,29 +3466,29 @@
       <c r="Q42" s="16"/>
       <c r="R42" s="16"/>
     </row>
-    <row r="43" spans="1:18" ht="36.75" customHeight="1">
+    <row r="43" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
-      <c r="B43" s="164" t="s">
+      <c r="B43" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="164"/>
-      <c r="D43" s="164"/>
-      <c r="E43" s="164"/>
-      <c r="F43" s="164"/>
-      <c r="G43" s="164"/>
-      <c r="H43" s="164"/>
-      <c r="I43" s="164"/>
-      <c r="J43" s="164"/>
-      <c r="K43" s="164"/>
-      <c r="L43" s="164"/>
-      <c r="M43" s="164"/>
-      <c r="N43" s="164"/>
-      <c r="O43" s="164"/>
-      <c r="P43" s="164"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="80"/>
+      <c r="I43" s="80"/>
+      <c r="J43" s="80"/>
+      <c r="K43" s="80"/>
+      <c r="L43" s="80"/>
+      <c r="M43" s="80"/>
+      <c r="N43" s="80"/>
+      <c r="O43" s="80"/>
+      <c r="P43" s="80"/>
       <c r="Q43" s="16"/>
       <c r="R43" s="16"/>
     </row>
-    <row r="44" spans="1:18" ht="9.75" customHeight="1">
+    <row r="44" spans="1:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="39"/>
       <c r="C44" s="16"/>
@@ -3497,227 +3508,227 @@
       <c r="Q44" s="16"/>
       <c r="R44" s="16"/>
     </row>
-    <row r="45" spans="1:18" ht="36.75" customHeight="1">
+    <row r="45" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
-      <c r="B45" s="136" t="s">
+      <c r="B45" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="136"/>
-      <c r="D45" s="136"/>
-      <c r="E45" s="136"/>
-      <c r="F45" s="136"/>
-      <c r="G45" s="136"/>
-      <c r="H45" s="136"/>
-      <c r="I45" s="136"/>
-      <c r="J45" s="136"/>
-      <c r="K45" s="136"/>
-      <c r="L45" s="136"/>
-      <c r="M45" s="136"/>
-      <c r="N45" s="136"/>
-      <c r="O45" s="136"/>
-      <c r="P45" s="136"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="79"/>
+      <c r="G45" s="79"/>
+      <c r="H45" s="79"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="79"/>
+      <c r="M45" s="79"/>
+      <c r="N45" s="79"/>
+      <c r="O45" s="79"/>
+      <c r="P45" s="79"/>
       <c r="Q45" s="16"/>
       <c r="R45" s="16"/>
     </row>
-    <row r="46" spans="1:18" ht="18" customHeight="1">
+    <row r="46" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
-      <c r="B46" s="137" t="s">
+      <c r="B46" s="123" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="137"/>
-      <c r="D46" s="137"/>
-      <c r="E46" s="137"/>
-      <c r="F46" s="137"/>
-      <c r="G46" s="137"/>
-      <c r="H46" s="137"/>
-      <c r="I46" s="137"/>
-      <c r="J46" s="137"/>
-      <c r="K46" s="137"/>
-      <c r="L46" s="137"/>
-      <c r="M46" s="137"/>
-      <c r="N46" s="137"/>
-      <c r="O46" s="137"/>
-      <c r="P46" s="137"/>
+      <c r="C46" s="123"/>
+      <c r="D46" s="123"/>
+      <c r="E46" s="123"/>
+      <c r="F46" s="123"/>
+      <c r="G46" s="123"/>
+      <c r="H46" s="123"/>
+      <c r="I46" s="123"/>
+      <c r="J46" s="123"/>
+      <c r="K46" s="123"/>
+      <c r="L46" s="123"/>
+      <c r="M46" s="123"/>
+      <c r="N46" s="123"/>
+      <c r="O46" s="123"/>
+      <c r="P46" s="123"/>
       <c r="Q46" s="16"/>
       <c r="R46" s="16"/>
     </row>
-    <row r="47" spans="1:18" ht="32.450000000000003" customHeight="1">
+    <row r="47" spans="1:18" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
-      <c r="B47" s="138" t="s">
+      <c r="B47" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="138"/>
-      <c r="D47" s="138"/>
-      <c r="E47" s="138"/>
-      <c r="F47" s="138"/>
-      <c r="G47" s="138"/>
-      <c r="H47" s="138"/>
-      <c r="I47" s="138"/>
-      <c r="J47" s="138"/>
-      <c r="K47" s="138"/>
-      <c r="L47" s="138"/>
-      <c r="M47" s="138"/>
-      <c r="N47" s="138"/>
-      <c r="O47" s="138"/>
-      <c r="P47" s="138"/>
+      <c r="C47" s="124"/>
+      <c r="D47" s="124"/>
+      <c r="E47" s="124"/>
+      <c r="F47" s="124"/>
+      <c r="G47" s="124"/>
+      <c r="H47" s="124"/>
+      <c r="I47" s="124"/>
+      <c r="J47" s="124"/>
+      <c r="K47" s="124"/>
+      <c r="L47" s="124"/>
+      <c r="M47" s="124"/>
+      <c r="N47" s="124"/>
+      <c r="O47" s="124"/>
+      <c r="P47" s="124"/>
       <c r="Q47" s="16"/>
       <c r="R47" s="16"/>
     </row>
-    <row r="48" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="48" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16"/>
-      <c r="B48" s="136" t="s">
+      <c r="B48" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="136"/>
-      <c r="D48" s="136"/>
-      <c r="E48" s="136"/>
-      <c r="F48" s="136"/>
-      <c r="G48" s="136"/>
-      <c r="H48" s="136"/>
-      <c r="I48" s="136"/>
-      <c r="J48" s="136"/>
-      <c r="K48" s="136"/>
-      <c r="L48" s="136"/>
-      <c r="M48" s="136"/>
-      <c r="N48" s="136"/>
-      <c r="O48" s="136"/>
-      <c r="P48" s="136"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="79"/>
+      <c r="E48" s="79"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="79"/>
+      <c r="H48" s="79"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="79"/>
+      <c r="M48" s="79"/>
+      <c r="N48" s="79"/>
+      <c r="O48" s="79"/>
+      <c r="P48" s="79"/>
       <c r="Q48" s="16"/>
       <c r="R48" s="16"/>
     </row>
-    <row r="49" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="49" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16"/>
-      <c r="B49" s="136" t="s">
+      <c r="B49" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="136"/>
-      <c r="D49" s="136"/>
-      <c r="E49" s="136"/>
-      <c r="F49" s="136"/>
-      <c r="G49" s="136"/>
-      <c r="H49" s="136"/>
-      <c r="I49" s="136"/>
-      <c r="J49" s="136"/>
-      <c r="K49" s="136"/>
-      <c r="L49" s="136"/>
-      <c r="M49" s="136"/>
-      <c r="N49" s="136"/>
-      <c r="O49" s="136"/>
-      <c r="P49" s="136"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="79"/>
+      <c r="E49" s="79"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="79"/>
+      <c r="H49" s="79"/>
+      <c r="I49" s="79"/>
+      <c r="J49" s="79"/>
+      <c r="K49" s="79"/>
+      <c r="L49" s="79"/>
+      <c r="M49" s="79"/>
+      <c r="N49" s="79"/>
+      <c r="O49" s="79"/>
+      <c r="P49" s="79"/>
       <c r="Q49" s="16"/>
       <c r="R49" s="16"/>
     </row>
-    <row r="50" spans="1:18" ht="16.899999999999999" customHeight="1">
+    <row r="50" spans="1:18" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16"/>
-      <c r="B50" s="136" t="s">
+      <c r="B50" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="136"/>
-      <c r="D50" s="136"/>
-      <c r="E50" s="136"/>
-      <c r="F50" s="136"/>
-      <c r="G50" s="136"/>
-      <c r="H50" s="136"/>
-      <c r="I50" s="136"/>
-      <c r="J50" s="136"/>
-      <c r="K50" s="136"/>
-      <c r="L50" s="136"/>
-      <c r="M50" s="136"/>
-      <c r="N50" s="136"/>
-      <c r="O50" s="136"/>
-      <c r="P50" s="136"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="79"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="79"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="79"/>
+      <c r="J50" s="79"/>
+      <c r="K50" s="79"/>
+      <c r="L50" s="79"/>
+      <c r="M50" s="79"/>
+      <c r="N50" s="79"/>
+      <c r="O50" s="79"/>
+      <c r="P50" s="79"/>
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
     </row>
-    <row r="51" spans="1:18" ht="18.600000000000001" customHeight="1">
+    <row r="51" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16"/>
-      <c r="B51" s="136" t="s">
+      <c r="B51" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="136"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="136"/>
-      <c r="F51" s="136"/>
-      <c r="G51" s="136"/>
-      <c r="H51" s="136"/>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
-      <c r="K51" s="136"/>
-      <c r="L51" s="136"/>
-      <c r="M51" s="136"/>
-      <c r="N51" s="136"/>
-      <c r="O51" s="136"/>
-      <c r="P51" s="136"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="79"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="79"/>
+      <c r="H51" s="79"/>
+      <c r="I51" s="79"/>
+      <c r="J51" s="79"/>
+      <c r="K51" s="79"/>
+      <c r="L51" s="79"/>
+      <c r="M51" s="79"/>
+      <c r="N51" s="79"/>
+      <c r="O51" s="79"/>
+      <c r="P51" s="79"/>
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
     </row>
-    <row r="52" spans="1:18" ht="18" customHeight="1">
+    <row r="52" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16"/>
-      <c r="B52" s="136" t="s">
+      <c r="B52" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="136"/>
-      <c r="D52" s="136"/>
-      <c r="E52" s="136"/>
-      <c r="F52" s="136"/>
-      <c r="G52" s="136"/>
-      <c r="H52" s="136"/>
-      <c r="I52" s="136"/>
-      <c r="J52" s="136"/>
-      <c r="K52" s="136"/>
-      <c r="L52" s="136"/>
-      <c r="M52" s="136"/>
-      <c r="N52" s="136"/>
-      <c r="O52" s="136"/>
-      <c r="P52" s="136"/>
+      <c r="C52" s="79"/>
+      <c r="D52" s="79"/>
+      <c r="E52" s="79"/>
+      <c r="F52" s="79"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="79"/>
+      <c r="K52" s="79"/>
+      <c r="L52" s="79"/>
+      <c r="M52" s="79"/>
+      <c r="N52" s="79"/>
+      <c r="O52" s="79"/>
+      <c r="P52" s="79"/>
       <c r="Q52" s="16"/>
       <c r="R52" s="16"/>
     </row>
-    <row r="53" spans="1:18" ht="31.9" customHeight="1">
+    <row r="53" spans="1:18" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16"/>
-      <c r="B53" s="136" t="s">
+      <c r="B53" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="136"/>
-      <c r="D53" s="136"/>
-      <c r="E53" s="136"/>
-      <c r="F53" s="136"/>
-      <c r="G53" s="136"/>
-      <c r="H53" s="136"/>
-      <c r="I53" s="136"/>
-      <c r="J53" s="136"/>
-      <c r="K53" s="136"/>
-      <c r="L53" s="136"/>
-      <c r="M53" s="136"/>
-      <c r="N53" s="136"/>
-      <c r="O53" s="136"/>
-      <c r="P53" s="136"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="79"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="79"/>
+      <c r="K53" s="79"/>
+      <c r="L53" s="79"/>
+      <c r="M53" s="79"/>
+      <c r="N53" s="79"/>
+      <c r="O53" s="79"/>
+      <c r="P53" s="79"/>
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
     </row>
-    <row r="54" spans="1:18" ht="33" customHeight="1">
+    <row r="54" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
-      <c r="B54" s="136" t="s">
+      <c r="B54" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="136"/>
-      <c r="D54" s="136"/>
-      <c r="E54" s="136"/>
-      <c r="F54" s="136"/>
-      <c r="G54" s="136"/>
-      <c r="H54" s="136"/>
-      <c r="I54" s="136"/>
-      <c r="J54" s="136"/>
-      <c r="K54" s="136"/>
-      <c r="L54" s="136"/>
-      <c r="M54" s="136"/>
-      <c r="N54" s="136"/>
-      <c r="O54" s="136"/>
-      <c r="P54" s="136"/>
+      <c r="C54" s="79"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="79"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="79"/>
+      <c r="J54" s="79"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="79"/>
+      <c r="N54" s="79"/>
+      <c r="O54" s="79"/>
+      <c r="P54" s="79"/>
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
     </row>
-    <row r="55" spans="1:18" ht="15.75" customHeight="1">
+    <row r="55" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16"/>
       <c r="B55" s="49"/>
       <c r="C55" s="49"/>
@@ -3737,7 +3748,7 @@
       <c r="Q55" s="16"/>
       <c r="R55" s="16"/>
     </row>
-    <row r="56" spans="1:18" ht="12.95" customHeight="1">
+    <row r="56" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
@@ -3757,29 +3768,29 @@
       <c r="Q56" s="16"/>
       <c r="R56" s="16"/>
     </row>
-    <row r="57" spans="1:18" ht="12.75" customHeight="1">
+    <row r="57" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>
-      <c r="B57" s="131" t="s">
+      <c r="B57" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="131"/>
-      <c r="D57" s="131"/>
-      <c r="E57" s="131"/>
-      <c r="F57" s="131"/>
-      <c r="G57" s="131"/>
-      <c r="H57" s="131"/>
-      <c r="I57" s="131"/>
-      <c r="J57" s="131"/>
-      <c r="K57" s="131"/>
-      <c r="L57" s="131"/>
-      <c r="M57" s="131"/>
-      <c r="N57" s="131"/>
-      <c r="O57" s="131"/>
-      <c r="P57" s="131"/>
+      <c r="C57" s="78"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="78"/>
+      <c r="F57" s="78"/>
+      <c r="G57" s="78"/>
+      <c r="H57" s="78"/>
+      <c r="I57" s="78"/>
+      <c r="J57" s="78"/>
+      <c r="K57" s="78"/>
+      <c r="L57" s="78"/>
+      <c r="M57" s="78"/>
+      <c r="N57" s="78"/>
+      <c r="O57" s="78"/>
+      <c r="P57" s="78"/>
       <c r="Q57" s="16"/>
       <c r="R57" s="16"/>
     </row>
-    <row r="58" spans="1:18" ht="12.75" customHeight="1">
+    <row r="58" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
       <c r="B58" s="50"/>
       <c r="C58" s="50"/>
@@ -3799,7 +3810,7 @@
       <c r="Q58" s="16"/>
       <c r="R58" s="16"/>
     </row>
-    <row r="59" spans="1:18" ht="5.0999999999999996" customHeight="1">
+    <row r="59" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16"/>
       <c r="B59" s="16"/>
       <c r="C59" s="16"/>
@@ -3808,9 +3819,9 @@
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
       <c r="H59" s="16"/>
-      <c r="I59" s="135"/>
-      <c r="J59" s="135"/>
-      <c r="K59" s="135"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="76"/>
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
@@ -3819,27 +3830,27 @@
       <c r="Q59" s="16"/>
       <c r="R59" s="16"/>
     </row>
-    <row r="60" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="60" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
-      <c r="B60" s="135"/>
-      <c r="C60" s="135"/>
-      <c r="D60" s="135"/>
-      <c r="E60" s="135"/>
-      <c r="F60" s="135"/>
+      <c r="B60" s="76"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="76"/>
       <c r="G60" s="16"/>
-      <c r="H60" s="135"/>
-      <c r="I60" s="135"/>
-      <c r="J60" s="135"/>
-      <c r="K60" s="135"/>
+      <c r="H60" s="76"/>
+      <c r="I60" s="76"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="76"/>
       <c r="L60" s="16"/>
-      <c r="M60" s="135"/>
-      <c r="N60" s="135"/>
-      <c r="O60" s="135"/>
-      <c r="P60" s="135"/>
+      <c r="M60" s="76"/>
+      <c r="N60" s="76"/>
+      <c r="O60" s="76"/>
+      <c r="P60" s="76"/>
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
     </row>
-    <row r="61" spans="1:18" ht="5.0999999999999996" customHeight="1">
+    <row r="61" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
       <c r="C61" s="16"/>
@@ -3859,27 +3870,27 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
     </row>
-    <row r="62" spans="1:18" ht="15.75">
+    <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="16"/>
-      <c r="B62" s="123"/>
-      <c r="C62" s="131"/>
-      <c r="D62" s="131"/>
-      <c r="E62" s="131"/>
-      <c r="F62" s="131"/>
-      <c r="G62" s="131"/>
-      <c r="H62" s="131"/>
-      <c r="I62" s="131"/>
-      <c r="J62" s="131"/>
-      <c r="K62" s="131"/>
-      <c r="L62" s="131"/>
-      <c r="M62" s="131"/>
-      <c r="N62" s="131"/>
-      <c r="O62" s="131"/>
-      <c r="P62" s="131"/>
+      <c r="B62" s="112"/>
+      <c r="C62" s="78"/>
+      <c r="D62" s="78"/>
+      <c r="E62" s="78"/>
+      <c r="F62" s="78"/>
+      <c r="G62" s="78"/>
+      <c r="H62" s="78"/>
+      <c r="I62" s="78"/>
+      <c r="J62" s="78"/>
+      <c r="K62" s="78"/>
+      <c r="L62" s="78"/>
+      <c r="M62" s="78"/>
+      <c r="N62" s="78"/>
+      <c r="O62" s="78"/>
+      <c r="P62" s="78"/>
       <c r="Q62" s="16"/>
       <c r="R62" s="16"/>
     </row>
-    <row r="63" spans="1:18" ht="16.149999999999999" customHeight="1">
+    <row r="63" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -3899,53 +3910,53 @@
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
     </row>
-    <row r="64" spans="1:18" ht="17.45" customHeight="1">
+    <row r="64" spans="1:18" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64"/>
-      <c r="B64" s="123" t="str">
+      <c r="B64" s="112" t="str">
         <f>Settings!$B$10&amp;" "&amp;Settings!$B$11&amp;", "&amp;Settings!$B$12&amp;IF(ISBLANK(Settings!$B$13),", ",", "&amp;Settings!$B$13&amp;", ")&amp;IF(ISBLANK(Settings!$B$14),"",""&amp;Settings!$B$14&amp;", ")&amp;Settings!$B$15</f>
         <v>1157 Cushman Ave., San Diego, County, CA, 92110</v>
       </c>
-      <c r="C64" s="123"/>
-      <c r="D64" s="123"/>
-      <c r="E64" s="123"/>
-      <c r="F64" s="123"/>
-      <c r="G64" s="123"/>
-      <c r="H64" s="123"/>
-      <c r="I64" s="123"/>
-      <c r="J64" s="123"/>
-      <c r="K64" s="123"/>
-      <c r="L64" s="123"/>
-      <c r="M64" s="123"/>
-      <c r="N64" s="123"/>
-      <c r="O64" s="123"/>
-      <c r="P64" s="123"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="112"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="112"/>
+      <c r="G64" s="112"/>
+      <c r="H64" s="112"/>
+      <c r="I64" s="112"/>
+      <c r="J64" s="112"/>
+      <c r="K64" s="112"/>
+      <c r="L64" s="112"/>
+      <c r="M64" s="112"/>
+      <c r="N64" s="112"/>
+      <c r="O64" s="112"/>
+      <c r="P64" s="112"/>
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
     </row>
-    <row r="65" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="65" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16"/>
-      <c r="B65" s="124" t="str">
+      <c r="B65" s="113" t="str">
         <f>"Tel: "&amp;Settings!$B$17&amp;" Fax: "&amp;Settings!$B$18&amp;IF(ISBLANK(Settings!$B$19)," "," E-mail: "&amp;Settings!$B$19)&amp;IF(ISBLANK(Settings!$B$20)," "," Web: "&amp;Settings!$B$20)</f>
         <v>Tel: 619-937-3961 Fax: 619-937-3965 E-mail: info@axisrg.com Web: www.axisrg.com</v>
       </c>
-      <c r="C65" s="124"/>
-      <c r="D65" s="124"/>
-      <c r="E65" s="124"/>
-      <c r="F65" s="124"/>
-      <c r="G65" s="124"/>
-      <c r="H65" s="124"/>
-      <c r="I65" s="124"/>
-      <c r="J65" s="124"/>
-      <c r="K65" s="124"/>
-      <c r="L65" s="124"/>
-      <c r="M65" s="124"/>
-      <c r="N65" s="124"/>
-      <c r="O65" s="124"/>
-      <c r="P65" s="124"/>
+      <c r="C65" s="113"/>
+      <c r="D65" s="113"/>
+      <c r="E65" s="113"/>
+      <c r="F65" s="113"/>
+      <c r="G65" s="113"/>
+      <c r="H65" s="113"/>
+      <c r="I65" s="113"/>
+      <c r="J65" s="113"/>
+      <c r="K65" s="113"/>
+      <c r="L65" s="113"/>
+      <c r="M65" s="113"/>
+      <c r="N65" s="113"/>
+      <c r="O65" s="113"/>
+      <c r="P65" s="113"/>
       <c r="Q65" s="16"/>
       <c r="R65" s="16"/>
     </row>
-    <row r="66" spans="1:18" ht="15.75">
+    <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="16"/>
@@ -3965,7 +3976,7 @@
       <c r="Q66" s="16"/>
       <c r="R66" s="16"/>
     </row>
-    <row r="67" spans="1:18" ht="15.75">
+    <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="16"/>
       <c r="B67" s="16"/>
       <c r="C67" s="16"/>
@@ -3985,57 +3996,44 @@
       <c r="Q67" s="16"/>
       <c r="R67" s="16"/>
     </row>
-    <row r="68" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="69" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="70" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="71" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="72" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="73" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="74" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="75" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="76" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="77" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="78" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="79" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="80" spans="1:18" ht="12.95" customHeight="1"/>
-    <row r="81" ht="12.95" customHeight="1"/>
-    <row r="82" ht="12.95" customHeight="1"/>
-    <row r="83" ht="12.95" customHeight="1"/>
-    <row r="84" ht="12.95" customHeight="1"/>
-    <row r="85" ht="12.95" customHeight="1"/>
-    <row r="86" ht="12.95" customHeight="1"/>
-    <row r="87" ht="12.95" customHeight="1"/>
+    <row r="68" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="M60:P60"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="B57:P57"/>
-    <mergeCell ref="B51:P51"/>
-    <mergeCell ref="B52:P52"/>
-    <mergeCell ref="B53:P53"/>
-    <mergeCell ref="B43:P43"/>
-    <mergeCell ref="B50:P50"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="M2:P3"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="I11:P15"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="B25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="I10:P10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="B12:E14"/>
+    <mergeCell ref="B22:L22"/>
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="B64:P64"/>
     <mergeCell ref="B65:P65"/>
@@ -4052,22 +4050,35 @@
     <mergeCell ref="B47:P47"/>
     <mergeCell ref="B48:P48"/>
     <mergeCell ref="B49:P49"/>
-    <mergeCell ref="M2:P3"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="I11:P15"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="B25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="I10:P10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="B12:E14"/>
-    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="M60:P60"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="B57:P57"/>
+    <mergeCell ref="B51:P51"/>
+    <mergeCell ref="B52:P52"/>
+    <mergeCell ref="B53:P53"/>
+    <mergeCell ref="B43:P43"/>
+    <mergeCell ref="B50:P50"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B31:L31">
@@ -4174,20 +4185,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>57</v>
       </c>
@@ -4195,7 +4206,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="47.25">
+    <row r="2" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
         <v>70</v>
       </c>
@@ -4203,7 +4214,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="38.25">
+    <row r="3" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="59" t="s">
         <v>58</v>
       </c>
@@ -4211,7 +4222,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="38.25">
+    <row r="4" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
         <v>60</v>
       </c>
@@ -4219,7 +4230,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="78.75">
+    <row r="5" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A5" s="60" t="s">
         <v>71</v>
       </c>
@@ -4227,7 +4238,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="38.25">
+    <row r="6" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="59" t="s">
         <v>59</v>
       </c>
@@ -4235,7 +4246,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
         <v>78</v>
       </c>
@@ -4243,7 +4254,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="59" t="s">
         <v>83</v>
       </c>
@@ -4251,23 +4262,23 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="61"/>
       <c r="C9" s="62" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>79</v>
       </c>

</xml_diff>